<commit_message>
se finaliza informe respecto a aprendizaje supervisado (SVM) y se da inicio a la tercera tarea (k-means)
</commit_message>
<xml_diff>
--- a/Tarea 2/enunciado_informe/f-score.xlsx
+++ b/Tarea 2/enunciado_informe/f-score.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="calculo" sheetId="1" r:id="rId1"/>
+    <sheet name="f-score" sheetId="2" r:id="rId2"/>
+    <sheet name="roc" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -21,7 +21,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0">
+    <comment ref="G2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -38,14 +38,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
+especifidad</t>
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0">
+    <comment ref="O2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,14 +62,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
+especifidad</t>
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="G16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,14 +86,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
+especifidad</t>
         </r>
       </text>
     </comment>
-    <comment ref="N14" authorId="0">
+    <comment ref="O16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,154 +110,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F32" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N32" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-no se ocupa para ninguna formula.</t>
+especifidad</t>
         </r>
       </text>
     </comment>
@@ -266,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="36">
   <si>
     <t>Classified Positive</t>
   </si>
@@ -304,9 +160,6 @@
     <t>world</t>
   </si>
   <si>
-    <t>useful</t>
-  </si>
-  <si>
     <t>split 01</t>
   </si>
   <si>
@@ -335,13 +188,55 @@
   </si>
   <si>
     <t>split 10</t>
+  </si>
+  <si>
+    <t>usa only</t>
+  </si>
+  <si>
+    <t>F-score</t>
+  </si>
+  <si>
+    <t>non-usa</t>
+  </si>
+  <si>
+    <t>clase</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>undet</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>non usa</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TPR</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>TNR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,12 +268,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
@@ -393,8 +282,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,13 +310,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,11 +335,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -444,19 +352,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -877,11 +790,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,15 +811,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="I1" s="7"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -920,9 +833,9 @@
       <c r="G2" s="2">
         <v>2</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>0</v>
@@ -955,7 +868,7 @@
       <c r="G3" s="2">
         <v>0</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="3" t="s">
         <v>3</v>
       </c>
@@ -984,16 +897,15 @@
       </c>
       <c r="D4" s="2">
         <f>G5</f>
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="2">
-        <f>11+5+11</f>
         <v>27</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1003,36 +915,33 @@
       </c>
       <c r="L4" s="2">
         <f>O5</f>
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O4" s="2">
-        <f>2+9+22</f>
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="N5" s="5" t="s">
+      <c r="G5" s="9">
+        <f>48+43+80</f>
+        <v>171</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="5"/>
+      <c r="N5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="O5" s="9">
+        <f>46+35+86</f>
+        <v>167</v>
+      </c>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -1043,7 +952,7 @@
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +972,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="I7" s="7"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1085,7 +994,7 @@
       </c>
       <c r="D8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1097,14 +1006,14 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I9" s="7"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I10" s="7"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>0</v>
@@ -1118,9 +1027,9 @@
       <c r="G11" s="2">
         <v>3</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>0</v>
@@ -1153,7 +1062,7 @@
       <c r="G12" s="2">
         <v>1</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1182,16 +1091,15 @@
       </c>
       <c r="D13" s="2">
         <f>G14</f>
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="2">
-        <f>6+8+21</f>
         <v>35</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="3" t="s">
         <v>5</v>
       </c>
@@ -1201,36 +1109,33 @@
       </c>
       <c r="L13" s="2">
         <f>O14</f>
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O13" s="2">
-        <f>10+21</f>
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="N14" s="5" t="s">
+      <c r="G14" s="9">
+        <f>46+32+83</f>
+        <v>161</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="5"/>
+      <c r="N14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O14" s="6">
-        <v>0</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="O14" s="9">
+        <f>39+43+82</f>
+        <v>164</v>
+      </c>
+      <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
@@ -1241,7 +1146,7 @@
         <v>7.8947368421052627E-2</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="3" t="s">
         <v>8</v>
       </c>
@@ -1261,7 +1166,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="I16" s="7"/>
+      <c r="I16" s="5"/>
       <c r="J16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1282,7 +1187,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="I17" s="7"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1294,14 +1199,14 @@
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="I18" s="7"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="I19" s="7"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>0</v>
@@ -1315,9 +1220,9 @@
       <c r="G20" s="2">
         <v>4</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>0</v>
@@ -1350,7 +1255,7 @@
       <c r="G21" s="2">
         <v>0</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="3" t="s">
         <v>3</v>
       </c>
@@ -1379,16 +1284,15 @@
       </c>
       <c r="D22" s="2">
         <f>G23</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="2">
-        <f>5+9+23</f>
         <v>37</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="3" t="s">
         <v>5</v>
       </c>
@@ -1398,36 +1302,33 @@
       </c>
       <c r="L22" s="2">
         <f>O23</f>
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O22" s="2">
-        <f>8+5+21</f>
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="6">
-        <v>0</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="N23" s="5" t="s">
+      <c r="G23" s="9">
+        <f>49+34+76</f>
+        <v>159</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="5"/>
+      <c r="N23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O23" s="6">
-        <v>0</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="O23" s="9">
+        <f>36+37+89</f>
+        <v>162</v>
+      </c>
+      <c r="P23" s="9"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
@@ -1438,7 +1339,7 @@
         <v>9.7560975609756101E-2</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="I24" s="7"/>
+      <c r="I24" s="5"/>
       <c r="J24" s="3" t="s">
         <v>8</v>
       </c>
@@ -1458,7 +1359,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="I25" s="7"/>
+      <c r="I25" s="5"/>
       <c r="J25" s="3" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1380,7 @@
       </c>
       <c r="D26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="I26" s="7"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="3" t="s">
         <v>10</v>
       </c>
@@ -1491,14 +1392,14 @@
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="I27" s="7"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="I28" s="7"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>0</v>
@@ -1512,9 +1413,9 @@
       <c r="G29" s="2">
         <v>7</v>
       </c>
-      <c r="I29" s="7"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>0</v>
@@ -1547,7 +1448,7 @@
       <c r="G30" s="2">
         <v>1</v>
       </c>
-      <c r="I30" s="7"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="3" t="s">
         <v>3</v>
       </c>
@@ -1576,16 +1477,15 @@
       </c>
       <c r="D31" s="2">
         <f>G32</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G31" s="2">
-        <f>9+5+18</f>
         <v>32</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="5"/>
       <c r="J31" s="3" t="s">
         <v>5</v>
       </c>
@@ -1595,36 +1495,33 @@
       </c>
       <c r="L31" s="2">
         <f>O32</f>
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O31" s="2">
-        <f>10+12+13</f>
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="6">
-        <v>0</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" s="7"/>
-      <c r="N32" s="5" t="s">
+      <c r="G32" s="9">
+        <f>47+34+79</f>
+        <v>160</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="5"/>
+      <c r="N32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O32" s="6">
-        <v>0</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="O32" s="9">
+        <f>45+30+87</f>
+        <v>162</v>
+      </c>
+      <c r="P32" s="9"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
@@ -1635,7 +1532,7 @@
         <v>0.17948717948717949</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="I33" s="7"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="3" t="s">
         <v>8</v>
       </c>
@@ -1655,7 +1552,7 @@
       </c>
       <c r="D34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="I34" s="7"/>
+      <c r="I34" s="5"/>
       <c r="J34" s="3" t="s">
         <v>9</v>
       </c>
@@ -1676,7 +1573,7 @@
       </c>
       <c r="D35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="I35" s="7"/>
+      <c r="I35" s="5"/>
       <c r="J35" s="3" t="s">
         <v>10</v>
       </c>
@@ -1688,14 +1585,14 @@
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="I36" s="7"/>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="I37" s="7"/>
+      <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>0</v>
@@ -1709,9 +1606,9 @@
       <c r="G38" s="2">
         <v>3</v>
       </c>
-      <c r="I38" s="7"/>
+      <c r="I38" s="5"/>
       <c r="J38" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>0</v>
@@ -1744,7 +1641,7 @@
       <c r="G39" s="2">
         <v>2</v>
       </c>
-      <c r="I39" s="7"/>
+      <c r="I39" s="5"/>
       <c r="J39" s="3" t="s">
         <v>3</v>
       </c>
@@ -1773,16 +1670,15 @@
       </c>
       <c r="D40" s="2">
         <f>G41</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G40" s="2">
-        <f>8+5+23</f>
         <v>36</v>
       </c>
-      <c r="I40" s="7"/>
+      <c r="I40" s="5"/>
       <c r="J40" s="3" t="s">
         <v>5</v>
       </c>
@@ -1792,36 +1688,33 @@
       </c>
       <c r="L40" s="2">
         <f>O41</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O40" s="2">
-        <f>9+7+19</f>
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G41" s="6">
-        <v>0</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I41" s="7"/>
-      <c r="N41" s="5" t="s">
+      <c r="G41" s="9">
+        <f>43+39+77</f>
+        <v>159</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="5"/>
+      <c r="N41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O41" s="6">
-        <v>0</v>
-      </c>
-      <c r="P41" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="O41" s="9">
+        <f>54+45+61</f>
+        <v>160</v>
+      </c>
+      <c r="P41" s="9"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
@@ -1832,7 +1725,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="I42" s="7"/>
+      <c r="I42" s="5"/>
       <c r="J42" s="3" t="s">
         <v>8</v>
       </c>
@@ -1852,7 +1745,7 @@
       </c>
       <c r="D43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="I43" s="7"/>
+      <c r="I43" s="5"/>
       <c r="J43" s="3" t="s">
         <v>9</v>
       </c>
@@ -1873,7 +1766,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="I44" s="7"/>
+      <c r="I44" s="5"/>
       <c r="J44" s="3" t="s">
         <v>10</v>
       </c>
@@ -1888,30 +1781,1573 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.78048780500000003</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.71061947000000003</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.29032258</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.855614973</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.14285714299999999</v>
+      </c>
+      <c r="M3" s="2">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.82178217799999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.72592592600000005</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.64761904800000003</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.177777778</v>
+      </c>
+      <c r="M4" s="2">
+        <v>3</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.80423280399999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.74015748000000003</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.67326732700000003</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.29787234000000001</v>
+      </c>
+      <c r="M5" s="2">
+        <v>4</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.82722513099999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.69354838699999999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.67241379300000004</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.13636363600000001</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.80208333300000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.67961165000000001</v>
+      </c>
+      <c r="I7" s="2">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>6</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.83902438999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.70909090900000005</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.728813559</v>
+      </c>
+      <c r="I8" s="2">
+        <v>7</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>7</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.836734694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.67924528299999998</v>
+      </c>
+      <c r="E9" s="2">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.68518518500000003</v>
+      </c>
+      <c r="I9" s="2">
+        <v>8</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.19047618999999999</v>
+      </c>
+      <c r="M9" s="2">
+        <v>8</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0.83962264200000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.71428571399999996</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="I10" s="2">
+        <v>9</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="M10" s="2">
+        <v>9</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.82857142900000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.71428571399999996</v>
+      </c>
+      <c r="I11" s="2">
+        <v>10</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.18181818199999999</v>
+      </c>
+      <c r="M11" s="2">
+        <v>10</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.77215189900000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>125</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <f>A3/(A3+D3)</f>
+        <v>0.81355932203389836</v>
+      </c>
+      <c r="F3">
+        <f>C3/(B3+C3)</f>
+        <v>0.11347517730496454</v>
+      </c>
+      <c r="G3">
+        <f>B3/(B3+C3)</f>
+        <v>0.88652482269503541</v>
+      </c>
+      <c r="I3">
+        <v>42</v>
+      </c>
+      <c r="J3">
+        <v>130</v>
+      </c>
+      <c r="K3">
+        <v>22</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <f>I3/(I3+L3)</f>
+        <v>0.8936170212765957</v>
+      </c>
+      <c r="N3">
+        <f>K3/(J3+K3)</f>
+        <v>0.14473684210526316</v>
+      </c>
+      <c r="O3">
+        <f>J3/(J3+K3)</f>
+        <v>0.85526315789473684</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>118</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E12" si="0">A4/(A4+D4)</f>
+        <v>0.88461538461538458</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F12" si="1">C4/(B4+C4)</f>
+        <v>0.20270270270270271</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G12" si="2">B4/(B4+C4)</f>
+        <v>0.79729729729729726</v>
+      </c>
+      <c r="I4">
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <v>132</v>
+      </c>
+      <c r="K4">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M12" si="3">I4/(I4+L4)</f>
+        <v>0.8</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N12" si="4">K4/(J4+K4)</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O12" si="5">J4/(J4+K4)</f>
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>114</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.90740740740740744</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.21917808219178081</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0.78082191780821919</v>
+      </c>
+      <c r="I5">
+        <v>34</v>
+      </c>
+      <c r="J5">
+        <v>129</v>
+      </c>
+      <c r="K5">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>0.79069767441860461</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>0.17834394904458598</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>0.82165605095541405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>120</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.8392857142857143</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I6">
+        <v>34</v>
+      </c>
+      <c r="J6">
+        <v>133</v>
+      </c>
+      <c r="K6">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>0.87179487179487181</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>0.82608695652173914</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <v>119</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.84313725490196079</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.20134228187919462</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0.79865771812080533</v>
+      </c>
+      <c r="I7">
+        <v>39</v>
+      </c>
+      <c r="J7">
+        <v>123</v>
+      </c>
+      <c r="K7">
+        <v>33</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>0.88636363636363635</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>0.21153846153846154</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>0.78846153846153844</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>121</v>
+      </c>
+      <c r="C8">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.20394736842105263</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0.79605263157894735</v>
+      </c>
+      <c r="I8">
+        <v>35</v>
+      </c>
+      <c r="J8">
+        <v>132</v>
+      </c>
+      <c r="K8">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>0.79545454545454541</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>0.84615384615384615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>129</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.79591836734693877</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.14569536423841059</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0.85430463576158944</v>
+      </c>
+      <c r="I9">
+        <v>43</v>
+      </c>
+      <c r="J9">
+        <v>125</v>
+      </c>
+      <c r="K9">
+        <v>32</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>0.20382165605095542</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>0.79617834394904463</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>130</v>
+      </c>
+      <c r="C10">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I10">
+        <v>37</v>
+      </c>
+      <c r="J10">
+        <v>129</v>
+      </c>
+      <c r="K10">
+        <v>29</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>0.88095238095238093</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>0.18354430379746836</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>0.81645569620253167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>119</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.1793103448275862</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0.82068965517241377</v>
+      </c>
+      <c r="I11">
+        <v>30</v>
+      </c>
+      <c r="J11">
+        <v>134</v>
+      </c>
+      <c r="K11">
+        <v>24</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>0.15189873417721519</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="5"/>
+        <v>0.84810126582278478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>54</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.19708029197080293</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0.8029197080291971</v>
+      </c>
+      <c r="I12">
+        <v>45</v>
+      </c>
+      <c r="J12">
+        <v>119</v>
+      </c>
+      <c r="K12">
+        <v>29</v>
+      </c>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>0.86538461538461542</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>0.19594594594594594</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="5"/>
+        <v>0.80405405405405406</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>93</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <f>A17/(A17+D17)</f>
+        <v>0.87912087912087911</v>
+      </c>
+      <c r="F17">
+        <f>C17/(B17+C17)</f>
+        <v>0.14678899082568808</v>
+      </c>
+      <c r="G17">
+        <f>B17/(B17+C17)</f>
+        <v>0.85321100917431192</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>171</v>
+      </c>
+      <c r="K17">
+        <v>27</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>I17/(I17+L17)</f>
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <f>K17/(J17+K17)</f>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="O17">
+        <f>J17/(J17+K17)</f>
+        <v>0.86363636363636365</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>83</v>
+      </c>
+      <c r="B18">
+        <v>81</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>21</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:E26" si="6">A18/(A18+D18)</f>
+        <v>0.79807692307692313</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ref="F18:F26" si="7">C18/(B18+C18)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G26" si="8">B18/(B18+C18)</f>
+        <v>0.84375</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>161</v>
+      </c>
+      <c r="K18">
+        <v>35</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M26" si="9">I18/(I18+L18)</f>
+        <v>0.75</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:N26" si="10">K18/(J18+K18)</f>
+        <v>0.17857142857142858</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18:O26" si="11">J18/(J18+K18)</f>
+        <v>0.8214285714285714</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>76</v>
+      </c>
+      <c r="B19">
+        <v>114</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>0.76767676767676762</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>0.109375</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="8"/>
+        <v>0.890625</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>159</v>
+      </c>
+      <c r="K19">
+        <v>37</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="10"/>
+        <v>0.18877551020408162</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="11"/>
+        <v>0.81122448979591832</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>79</v>
+      </c>
+      <c r="B20">
+        <v>88</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="6"/>
+        <v>0.81443298969072164</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>0.14563106796116504</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="8"/>
+        <v>0.85436893203883491</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>160</v>
+      </c>
+      <c r="K20">
+        <v>32</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="9"/>
+        <v>0.875</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="11"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>77</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>23</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="6"/>
+        <v>0.77</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>159</v>
+      </c>
+      <c r="K21">
+        <v>36</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="10"/>
+        <v>0.18461538461538463</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="11"/>
+        <v>0.81538461538461537</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>86</v>
+      </c>
+      <c r="B22">
+        <v>81</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="6"/>
+        <v>0.79629629629629628</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="7"/>
+        <v>0.11956521739130435</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="8"/>
+        <v>0.88043478260869568</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>167</v>
+      </c>
+      <c r="K22">
+        <v>33</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="10"/>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="11"/>
+        <v>0.83499999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>82</v>
+      </c>
+      <c r="B23">
+        <v>86</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="6"/>
+        <v>0.79611650485436891</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="7"/>
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="8"/>
+        <v>0.88659793814432986</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>164</v>
+      </c>
+      <c r="K23">
+        <v>31</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="9"/>
+        <v>0.8</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="10"/>
+        <v>0.15897435897435896</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="11"/>
+        <v>0.84102564102564104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>89</v>
+      </c>
+      <c r="B24">
+        <v>77</v>
+      </c>
+      <c r="C24">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>21</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>0.80909090909090908</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="7"/>
+        <v>0.14444444444444443</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="8"/>
+        <v>0.85555555555555551</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>162</v>
+      </c>
+      <c r="K24">
+        <v>34</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="10"/>
+        <v>0.17346938775510204</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="11"/>
+        <v>0.82653061224489799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>87</v>
+      </c>
+      <c r="B25">
+        <v>77</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>13</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>0.87</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="7"/>
+        <v>0.23</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="8"/>
+        <v>0.77</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>162</v>
+      </c>
+      <c r="K25">
+        <v>35</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="9"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="10"/>
+        <v>0.17766497461928935</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="11"/>
+        <v>0.82233502538071068</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>61</v>
+      </c>
+      <c r="B26">
+        <v>103</v>
+      </c>
+      <c r="C26">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="6"/>
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="7"/>
+        <v>0.2076923076923077</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="8"/>
+        <v>0.79230769230769227</v>
+      </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
+      <c r="J26">
+        <v>160</v>
+      </c>
+      <c r="K26">
+        <v>35</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="9"/>
+        <v>0.8</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="10"/>
+        <v>0.17948717948717949</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="11"/>
+        <v>0.82051282051282048</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>